<commit_message>
KPI Dashboard - data transfer XLS: create measurement
</commit_message>
<xml_diff>
--- a/excel-import/metricsimport.xlsx
+++ b/excel-import/metricsimport.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="24030" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="metricsimport" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Host</t>
   </si>
@@ -43,9 +44,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>ODhVGFcsg4tFPfntsKygHF3thH9WPmUfAUL2d2rh cdc95a97-6e85-4c31-9d28-230018d40671</t>
-  </si>
-  <si>
     <t>Measurement_Test</t>
   </si>
   <si>
@@ -68,6 +66,12 @@
   </si>
   <si>
     <t>Wert</t>
+  </si>
+  <si>
+    <t>ODhVGFcsg4tFPfntsKygHF3thH9WPmUfAUL2d2rh</t>
+  </si>
+  <si>
+    <t>cdc95a97-6e85-4c31-9d28-230018d40671</t>
   </si>
 </sst>
 </file>
@@ -75,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -557,7 +561,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -957,31 +961,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>42815.551388888889</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -989,31 +996,34 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>42815.551388888889</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KPI Dashboard - data transfer XLS: the first draft
</commit_message>
<xml_diff>
--- a/excel-import/metricsimport.xlsx
+++ b/excel-import/metricsimport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="24030" windowHeight="10590"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="28620" windowHeight="2805"/>
   </bookViews>
   <sheets>
     <sheet name="metricsimport" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -568,6 +568,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -917,8 +924,8 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +935,7 @@
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -952,7 +960,16 @@
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -978,8 +995,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
+      <c r="H2" s="6">
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
@@ -1013,8 +1030,8 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
+      <c r="H3" s="6">
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>10</v>
@@ -1022,8 +1039,8 @@
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>16</v>
+      <c r="K3" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>